<commit_message>
practice pushing to github
</commit_message>
<xml_diff>
--- a/march10_pravda.xlsx
+++ b/march10_pravda.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegrubbs/Desktop/GitHub/NAV_Capstone/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681F7BBB-5111-1040-BE5C-6FD3818AF329}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pravda_Scraped" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1129,8 +1135,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1206,6 +1212,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1252,7 +1266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1284,9 +1298,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1318,6 +1350,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1493,14 +1543,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2394</v>
       </c>
@@ -1546,16 +1601,16 @@
         <v>347</v>
       </c>
       <c r="G2">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H2">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>8155</v>
       </c>
@@ -1575,16 +1630,16 @@
         <v>348</v>
       </c>
       <c r="G3">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H3">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I3" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>9432</v>
       </c>
@@ -1604,16 +1659,16 @@
         <v>347</v>
       </c>
       <c r="G4">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H4">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I4" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>10488</v>
       </c>
@@ -1633,16 +1688,16 @@
         <v>348</v>
       </c>
       <c r="G5">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H5">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I5" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14559</v>
       </c>
@@ -1662,16 +1717,16 @@
         <v>347</v>
       </c>
       <c r="G6">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H6">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I6" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>16835</v>
       </c>
@@ -1691,16 +1746,16 @@
         <v>347</v>
       </c>
       <c r="G7">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H7">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I7" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>20028</v>
       </c>
@@ -1717,16 +1772,16 @@
         <v>343</v>
       </c>
       <c r="G8">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H8">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I8" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>28047</v>
       </c>
@@ -1746,16 +1801,16 @@
         <v>347</v>
       </c>
       <c r="G9">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H9">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I9" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>39231</v>
       </c>
@@ -1775,16 +1830,16 @@
         <v>348</v>
       </c>
       <c r="G10">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H10">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I10" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>49853</v>
       </c>
@@ -1801,16 +1856,16 @@
         <v>343</v>
       </c>
       <c r="G11">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H11">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>58619</v>
       </c>
@@ -1830,16 +1885,16 @@
         <v>349</v>
       </c>
       <c r="G12">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H12">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I12" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>72391</v>
       </c>
@@ -1859,16 +1914,16 @@
         <v>350</v>
       </c>
       <c r="G13">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H13">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I13" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>73212</v>
       </c>
@@ -1888,16 +1943,16 @@
         <v>348</v>
       </c>
       <c r="G14">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H14">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I14" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>82589</v>
       </c>
@@ -1917,16 +1972,16 @@
         <v>350</v>
       </c>
       <c r="G15">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H15">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I15" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>89151</v>
       </c>
@@ -1946,16 +2001,16 @@
         <v>348</v>
       </c>
       <c r="G16">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H16">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I16" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>107505</v>
       </c>
@@ -1972,16 +2027,16 @@
         <v>343</v>
       </c>
       <c r="G17">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H17">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I17" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>118230</v>
       </c>
@@ -2001,16 +2056,16 @@
         <v>347</v>
       </c>
       <c r="G18">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H18">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I18" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>123090</v>
       </c>
@@ -2027,16 +2082,16 @@
         <v>343</v>
       </c>
       <c r="G19">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H19">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I19" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>126196</v>
       </c>
@@ -2056,16 +2111,16 @@
         <v>351</v>
       </c>
       <c r="G20">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H20">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I20" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>151630</v>
       </c>
@@ -2085,16 +2140,16 @@
         <v>352</v>
       </c>
       <c r="G21">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H21">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I21" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>157019</v>
       </c>
@@ -2114,16 +2169,16 @@
         <v>348</v>
       </c>
       <c r="G22">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H22">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I22" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>171531</v>
       </c>
@@ -2143,16 +2198,16 @@
         <v>348</v>
       </c>
       <c r="G23">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H23">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I23" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>185385</v>
       </c>
@@ -2172,16 +2227,16 @@
         <v>348</v>
       </c>
       <c r="G24">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H24">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I24" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>190624</v>
       </c>
@@ -2198,16 +2253,16 @@
         <v>343</v>
       </c>
       <c r="G25">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H25">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I25" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>202446</v>
       </c>
@@ -2227,16 +2282,16 @@
         <v>353</v>
       </c>
       <c r="G26">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H26">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I26" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>208499</v>
       </c>
@@ -2256,16 +2311,16 @@
         <v>347</v>
       </c>
       <c r="G27">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H27">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I27" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>232654</v>
       </c>
@@ -2285,16 +2340,16 @@
         <v>348</v>
       </c>
       <c r="G28">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H28">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>233274</v>
       </c>
@@ -2314,16 +2369,16 @@
         <v>354</v>
       </c>
       <c r="G29">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H29">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I29" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>239949</v>
       </c>
@@ -2343,16 +2398,16 @@
         <v>355</v>
       </c>
       <c r="G30">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H30">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I30" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>241104</v>
       </c>
@@ -2369,16 +2424,16 @@
         <v>343</v>
       </c>
       <c r="G31">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H31">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I31" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>247266</v>
       </c>
@@ -2395,16 +2450,16 @@
         <v>343</v>
       </c>
       <c r="G32">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H32">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I32" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>251469</v>
       </c>
@@ -2421,16 +2476,16 @@
         <v>343</v>
       </c>
       <c r="G33">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H33">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I33" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>254991</v>
       </c>
@@ -2450,16 +2505,16 @@
         <v>348</v>
       </c>
       <c r="G34">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H34">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I34" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>258541</v>
       </c>
@@ -2479,16 +2534,16 @@
         <v>348</v>
       </c>
       <c r="G35">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H35">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I35" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>259030</v>
       </c>
@@ -2508,16 +2563,16 @@
         <v>347</v>
       </c>
       <c r="G36">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H36">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I36" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>261333</v>
       </c>
@@ -2537,16 +2592,16 @@
         <v>356</v>
       </c>
       <c r="G37">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H37">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I37" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>272368</v>
       </c>
@@ -2566,16 +2621,16 @@
         <v>347</v>
       </c>
       <c r="G38">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H38">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I38" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>281071</v>
       </c>
@@ -2595,16 +2650,16 @@
         <v>348</v>
       </c>
       <c r="G39">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H39">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I39" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>283524</v>
       </c>
@@ -2624,16 +2679,16 @@
         <v>347</v>
       </c>
       <c r="G40">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H40">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I40" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>284718</v>
       </c>
@@ -2650,16 +2705,16 @@
         <v>343</v>
       </c>
       <c r="G41">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H41">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I41" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>295678</v>
       </c>
@@ -2679,16 +2734,16 @@
         <v>348</v>
       </c>
       <c r="G42">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H42">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I42" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>301928</v>
       </c>
@@ -2708,16 +2763,16 @@
         <v>348</v>
       </c>
       <c r="G43">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H43">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I43" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>336793</v>
       </c>
@@ -2737,16 +2792,16 @@
         <v>357</v>
       </c>
       <c r="G44">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H44">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I44" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>347004</v>
       </c>
@@ -2766,16 +2821,16 @@
         <v>358</v>
       </c>
       <c r="G45">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H45">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I45" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>356547</v>
       </c>
@@ -2792,16 +2847,16 @@
         <v>343</v>
       </c>
       <c r="G46">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H46">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I46" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>357457</v>
       </c>
@@ -2821,16 +2876,16 @@
         <v>348</v>
       </c>
       <c r="G47">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H47">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I47" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>358192</v>
       </c>
@@ -2850,16 +2905,16 @@
         <v>350</v>
       </c>
       <c r="G48">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H48">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I48" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>363684</v>
       </c>
@@ -2879,16 +2934,16 @@
         <v>356</v>
       </c>
       <c r="G49">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H49">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I49" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>365151</v>
       </c>
@@ -2908,16 +2963,16 @@
         <v>348</v>
       </c>
       <c r="G50">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H50">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I50" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>377065</v>
       </c>
@@ -2937,16 +2992,16 @@
         <v>359</v>
       </c>
       <c r="G51">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H51">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I51" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>386405</v>
       </c>
@@ -2966,16 +3021,16 @@
         <v>360</v>
       </c>
       <c r="G52">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H52">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I52" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>386890</v>
       </c>
@@ -2995,16 +3050,16 @@
         <v>360</v>
       </c>
       <c r="G53">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H53">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I53" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>389202</v>
       </c>
@@ -3024,16 +3079,16 @@
         <v>360</v>
       </c>
       <c r="G54">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H54">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I54" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>414755</v>
       </c>
@@ -3053,16 +3108,16 @@
         <v>348</v>
       </c>
       <c r="G55">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H55">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I55" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>425679</v>
       </c>
@@ -3082,16 +3137,16 @@
         <v>361</v>
       </c>
       <c r="G56">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H56">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I56" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>430573</v>
       </c>
@@ -3111,16 +3166,16 @@
         <v>348</v>
       </c>
       <c r="G57">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H57">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I57" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>441884</v>
       </c>
@@ -3137,16 +3192,16 @@
         <v>343</v>
       </c>
       <c r="G58">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H58">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I58" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>443264</v>
       </c>
@@ -3163,16 +3218,16 @@
         <v>343</v>
       </c>
       <c r="G59">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H59">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I59" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>452169</v>
       </c>
@@ -3192,16 +3247,16 @@
         <v>348</v>
       </c>
       <c r="G60">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H60">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I60" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>453886</v>
       </c>
@@ -3221,16 +3276,16 @@
         <v>347</v>
       </c>
       <c r="G61">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H61">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I61" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>458469</v>
       </c>
@@ -3250,16 +3305,16 @@
         <v>351</v>
       </c>
       <c r="G62">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H62">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I62" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>460318</v>
       </c>
@@ -3279,16 +3334,16 @@
         <v>347</v>
       </c>
       <c r="G63">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H63">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I63" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>464690</v>
       </c>
@@ -3308,16 +3363,16 @@
         <v>353</v>
       </c>
       <c r="G64">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H64">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I64" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>482057</v>
       </c>
@@ -3337,16 +3392,16 @@
         <v>348</v>
       </c>
       <c r="G65">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H65">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I65" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>483897</v>
       </c>
@@ -3366,16 +3421,16 @@
         <v>351</v>
       </c>
       <c r="G66">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H66">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I66" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>485566</v>
       </c>
@@ -3395,16 +3450,16 @@
         <v>350</v>
       </c>
       <c r="G67">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H67">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I67" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>487444</v>
       </c>
@@ -3424,16 +3479,16 @@
         <v>348</v>
       </c>
       <c r="G68">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H68">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I68" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>498678</v>
       </c>
@@ -3453,16 +3508,16 @@
         <v>347</v>
       </c>
       <c r="G69">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H69">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I69" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>499341</v>
       </c>
@@ -3479,16 +3534,16 @@
         <v>343</v>
       </c>
       <c r="G70">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H70">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I70" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>505108</v>
       </c>
@@ -3508,16 +3563,16 @@
         <v>348</v>
       </c>
       <c r="G71">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H71">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I71" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>508729</v>
       </c>
@@ -3534,16 +3589,16 @@
         <v>343</v>
       </c>
       <c r="G72">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H72">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I72" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>513673</v>
       </c>
@@ -3560,16 +3615,16 @@
         <v>343</v>
       </c>
       <c r="G73">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H73">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I73" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>520346</v>
       </c>
@@ -3586,16 +3641,16 @@
         <v>343</v>
       </c>
       <c r="G74">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H74">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I74" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>520674</v>
       </c>
@@ -3615,16 +3670,16 @@
         <v>347</v>
       </c>
       <c r="G75">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H75">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I75" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>527865</v>
       </c>
@@ -3644,16 +3699,16 @@
         <v>352</v>
       </c>
       <c r="G76">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H76">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I76" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>531039</v>
       </c>
@@ -3673,16 +3728,16 @@
         <v>348</v>
       </c>
       <c r="G77">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H77">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I77" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>550389</v>
       </c>
@@ -3702,16 +3757,16 @@
         <v>362</v>
       </c>
       <c r="G78">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H78">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I78" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>552591</v>
       </c>
@@ -3731,16 +3786,16 @@
         <v>347</v>
       </c>
       <c r="G79">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H79">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I79" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>588747</v>
       </c>
@@ -3760,16 +3815,16 @@
         <v>348</v>
       </c>
       <c r="G80">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H80">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I80" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>590435</v>
       </c>
@@ -3789,16 +3844,16 @@
         <v>348</v>
       </c>
       <c r="G81">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H81">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I81" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>592401</v>
       </c>
@@ -3818,16 +3873,16 @@
         <v>348</v>
       </c>
       <c r="G82">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H82">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I82" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>620889</v>
       </c>
@@ -3844,16 +3899,16 @@
         <v>343</v>
       </c>
       <c r="G83">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H83">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I83" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>623508</v>
       </c>
@@ -3873,16 +3928,16 @@
         <v>348</v>
       </c>
       <c r="G84">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H84">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I84" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>625953</v>
       </c>
@@ -3902,16 +3957,16 @@
         <v>351</v>
       </c>
       <c r="G85">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H85">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I85" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>631806</v>
       </c>
@@ -3931,16 +3986,16 @@
         <v>363</v>
       </c>
       <c r="G86">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H86">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I86" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>635814</v>
       </c>
@@ -3960,16 +4015,16 @@
         <v>351</v>
       </c>
       <c r="G87">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H87">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I87" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>638692</v>
       </c>
@@ -3989,16 +4044,16 @@
         <v>360</v>
       </c>
       <c r="G88">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H88">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I88" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>639111</v>
       </c>
@@ -4018,16 +4073,16 @@
         <v>347</v>
       </c>
       <c r="G89">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H89">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I89" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>639348</v>
       </c>
@@ -4047,16 +4102,16 @@
         <v>347</v>
       </c>
       <c r="G90">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H90">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I90" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>654389</v>
       </c>
@@ -4076,16 +4131,16 @@
         <v>347</v>
       </c>
       <c r="G91">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H91">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I91" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>655125</v>
       </c>
@@ -4105,16 +4160,16 @@
         <v>364</v>
       </c>
       <c r="G92">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H92">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I92" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>668126</v>
       </c>
@@ -4131,16 +4186,16 @@
         <v>343</v>
       </c>
       <c r="G93">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H93">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I93" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>720804</v>
       </c>
@@ -4160,16 +4215,16 @@
         <v>347</v>
       </c>
       <c r="G94">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H94">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I94" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>729011</v>
       </c>
@@ -4189,16 +4244,16 @@
         <v>348</v>
       </c>
       <c r="G95">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H95">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I95" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>743436</v>
       </c>
@@ -4218,16 +4273,16 @@
         <v>352</v>
       </c>
       <c r="G96">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H96">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I96" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>743856</v>
       </c>
@@ -4247,16 +4302,16 @@
         <v>365</v>
       </c>
       <c r="G97">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H97">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I97" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>745799</v>
       </c>
@@ -4276,16 +4331,16 @@
         <v>348</v>
       </c>
       <c r="G98">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H98">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I98" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>748750</v>
       </c>
@@ -4302,16 +4357,16 @@
         <v>343</v>
       </c>
       <c r="G99">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H99">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I99" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>749258</v>
       </c>
@@ -4328,16 +4383,16 @@
         <v>343</v>
       </c>
       <c r="G100">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H100">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I100" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>750148</v>
       </c>
@@ -4354,16 +4409,16 @@
         <v>343</v>
       </c>
       <c r="G101">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H101">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I101" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>753972</v>
       </c>
@@ -4380,16 +4435,16 @@
         <v>343</v>
       </c>
       <c r="G102">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H102">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I102" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>761421</v>
       </c>
@@ -4409,16 +4464,16 @@
         <v>351</v>
       </c>
       <c r="G103">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H103">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I103" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>767811</v>
       </c>
@@ -4438,16 +4493,16 @@
         <v>348</v>
       </c>
       <c r="G104">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H104">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I104" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>770565</v>
       </c>
@@ -4464,16 +4519,16 @@
         <v>343</v>
       </c>
       <c r="G105">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H105">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I105" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>775823</v>
       </c>
@@ -4493,16 +4548,16 @@
         <v>360</v>
       </c>
       <c r="G106">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H106">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I106" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>776580</v>
       </c>
@@ -4522,16 +4577,16 @@
         <v>360</v>
       </c>
       <c r="G107">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H107">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I107" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>797347</v>
       </c>
@@ -4551,16 +4606,16 @@
         <v>348</v>
       </c>
       <c r="G108">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H108">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I108" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>798589</v>
       </c>
@@ -4577,16 +4632,16 @@
         <v>343</v>
       </c>
       <c r="G109">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H109">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I109" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>803690</v>
       </c>
@@ -4603,16 +4658,16 @@
         <v>343</v>
       </c>
       <c r="G110">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H110">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I110" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>806623</v>
       </c>
@@ -4632,16 +4687,16 @@
         <v>348</v>
       </c>
       <c r="G111">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H111">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I111" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>811031</v>
       </c>
@@ -4661,10 +4716,10 @@
         <v>348</v>
       </c>
       <c r="G112">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H112">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I112" t="s">
         <v>368</v>
@@ -4672,117 +4727,117 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
-    <hyperlink ref="B48" r:id="rId47"/>
-    <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53"/>
-    <hyperlink ref="B55" r:id="rId54"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B64" r:id="rId63"/>
-    <hyperlink ref="B65" r:id="rId64"/>
-    <hyperlink ref="B66" r:id="rId65"/>
-    <hyperlink ref="B67" r:id="rId66"/>
-    <hyperlink ref="B68" r:id="rId67"/>
-    <hyperlink ref="B69" r:id="rId68"/>
-    <hyperlink ref="B70" r:id="rId69"/>
-    <hyperlink ref="B71" r:id="rId70"/>
-    <hyperlink ref="B72" r:id="rId71"/>
-    <hyperlink ref="B73" r:id="rId72"/>
-    <hyperlink ref="B74" r:id="rId73"/>
-    <hyperlink ref="B75" r:id="rId74"/>
-    <hyperlink ref="B76" r:id="rId75"/>
-    <hyperlink ref="B77" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78"/>
-    <hyperlink ref="B80" r:id="rId79"/>
-    <hyperlink ref="B81" r:id="rId80"/>
-    <hyperlink ref="B82" r:id="rId81"/>
-    <hyperlink ref="B83" r:id="rId82"/>
-    <hyperlink ref="B84" r:id="rId83"/>
-    <hyperlink ref="B85" r:id="rId84"/>
-    <hyperlink ref="B86" r:id="rId85"/>
-    <hyperlink ref="B87" r:id="rId86"/>
-    <hyperlink ref="B88" r:id="rId87"/>
-    <hyperlink ref="B89" r:id="rId88"/>
-    <hyperlink ref="B90" r:id="rId89"/>
-    <hyperlink ref="B91" r:id="rId90"/>
-    <hyperlink ref="B92" r:id="rId91"/>
-    <hyperlink ref="B93" r:id="rId92"/>
-    <hyperlink ref="B94" r:id="rId93"/>
-    <hyperlink ref="B95" r:id="rId94"/>
-    <hyperlink ref="B96" r:id="rId95"/>
-    <hyperlink ref="B97" r:id="rId96"/>
-    <hyperlink ref="B98" r:id="rId97"/>
-    <hyperlink ref="B99" r:id="rId98"/>
-    <hyperlink ref="B100" r:id="rId99"/>
-    <hyperlink ref="B101" r:id="rId100"/>
-    <hyperlink ref="B102" r:id="rId101"/>
-    <hyperlink ref="B103" r:id="rId102"/>
-    <hyperlink ref="B104" r:id="rId103"/>
-    <hyperlink ref="B105" r:id="rId104"/>
-    <hyperlink ref="B106" r:id="rId105"/>
-    <hyperlink ref="B107" r:id="rId106"/>
-    <hyperlink ref="B108" r:id="rId107"/>
-    <hyperlink ref="B109" r:id="rId108"/>
-    <hyperlink ref="B110" r:id="rId109"/>
-    <hyperlink ref="B111" r:id="rId110"/>
-    <hyperlink ref="B112" r:id="rId111"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B108" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B109" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B110" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B111" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B112" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>